<commit_message>
clustering: add identity for data
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -4498,7 +4498,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4524,12 +4524,6 @@
       <sz val="10"/>
       <color rgb="FF1155cc"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -4607,13 +4601,13 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -8845,7 +8839,7 @@
       <c r="AY42" s="3"/>
       <c r="AZ42" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="377.25" customFormat="1" s="1">
       <c r="A43" s="2">
         <v>44661.87734953704</v>
       </c>
@@ -8927,7 +8921,7 @@
       <c r="AY43" s="3"/>
       <c r="AZ43" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="253.5" customFormat="1" s="1">
       <c r="A44" s="2">
         <v>44661.88207175926</v>
       </c>
@@ -9009,7 +9003,7 @@
       <c r="AY44" s="3"/>
       <c r="AZ44" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="467.25" customFormat="1" s="1">
       <c r="A45" s="2">
         <v>44661.89346064815</v>
       </c>
@@ -9091,7 +9085,7 @@
       <c r="AY45" s="3"/>
       <c r="AZ45" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="332.25" customFormat="1" s="1">
       <c r="A46" s="2">
         <v>44661.91300925926</v>
       </c>
@@ -9175,7 +9169,7 @@
       <c r="AY46" s="3"/>
       <c r="AZ46" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="107.25" customFormat="1" s="1">
       <c r="A47" s="2">
         <v>44661.99429398148</v>
       </c>
@@ -9259,7 +9253,7 @@
       <c r="AY47" s="3"/>
       <c r="AZ47" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="208.5" customFormat="1" s="1">
       <c r="A48" s="2">
         <v>44662.46576388889</v>
       </c>
@@ -9339,7 +9333,7 @@
       <c r="AY48" s="3"/>
       <c r="AZ48" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="107.25" customFormat="1" s="1">
       <c r="A49" s="2">
         <v>44662.556296296294</v>
       </c>
@@ -9421,7 +9415,7 @@
       <c r="AY49" s="3"/>
       <c r="AZ49" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="861" customFormat="1" s="1">
       <c r="A50" s="2">
         <v>44662.921747685185</v>
       </c>
@@ -9503,7 +9497,7 @@
       <c r="AY50" s="3"/>
       <c r="AZ50" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="591" customFormat="1" s="1">
       <c r="A51" s="2">
         <v>44663.46912037037</v>
       </c>
@@ -9585,7 +9579,7 @@
       <c r="AY51" s="3"/>
       <c r="AZ51" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="163.5" customFormat="1" s="1">
       <c r="A52" s="2">
         <v>44663.75908564815</v>
       </c>
@@ -9667,7 +9661,7 @@
       <c r="AY52" s="3"/>
       <c r="AZ52" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="557.25" customFormat="1" s="1">
       <c r="A53" s="2">
         <v>44663.89796296296</v>
       </c>
@@ -9747,7 +9741,7 @@
       <c r="AY53" s="3"/>
       <c r="AZ53" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="759.75" customFormat="1" s="1">
       <c r="A54" s="2">
         <v>44663.90766203704</v>
       </c>
@@ -9831,7 +9825,7 @@
       <c r="AY54" s="3"/>
       <c r="AZ54" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="141" customFormat="1" s="1">
       <c r="A55" s="2">
         <v>44663.916597222225</v>
       </c>
@@ -9913,7 +9907,7 @@
       <c r="AY55" s="3"/>
       <c r="AZ55" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="343.5" customFormat="1" s="1">
       <c r="A56" s="2">
         <v>44663.92427083333</v>
       </c>
@@ -9997,7 +9991,7 @@
       <c r="AY56" s="3"/>
       <c r="AZ56" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="197.25" customFormat="1" s="1">
       <c r="A57" s="2">
         <v>44664.02513888889</v>
       </c>
@@ -10081,7 +10075,7 @@
       <c r="AY57" s="3"/>
       <c r="AZ57" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="332.25" customFormat="1" s="1">
       <c r="A58" s="2">
         <v>44664.72607638889</v>
       </c>
@@ -10163,7 +10157,7 @@
       <c r="AY58" s="3"/>
       <c r="AZ58" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="366" customFormat="1" s="1">
       <c r="A59" s="2">
         <v>44664.75571759259</v>
       </c>
@@ -10247,7 +10241,7 @@
       <c r="AY59" s="3"/>
       <c r="AZ59" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="748.5" customFormat="1" s="1">
       <c r="A60" s="2">
         <v>44664.803125</v>
       </c>
@@ -10331,7 +10325,7 @@
       <c r="AY60" s="3"/>
       <c r="AZ60" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="613.5" customFormat="1" s="1">
       <c r="A61" s="2">
         <v>44664.999710648146</v>
       </c>
@@ -10407,7 +10401,7 @@
       <c r="AY61" s="3"/>
       <c r="AZ61" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="253.5" customFormat="1" s="1">
       <c r="A62" s="2">
         <v>44665.467453703706</v>
       </c>
@@ -10487,7 +10481,7 @@
       <c r="AY62" s="3"/>
       <c r="AZ62" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="242.25" customFormat="1" s="1">
       <c r="A63" s="2">
         <v>44667.02175925926</v>
       </c>
@@ -10569,7 +10563,7 @@
       <c r="AY63" s="3"/>
       <c r="AZ63" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="17.25" hidden="1">
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="28.5">
       <c r="A64" s="8">
         <v>44668.51908564815</v>
       </c>
@@ -10653,7 +10647,7 @@
       <c r="AY64" s="3"/>
       <c r="AZ64" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="17.25" hidden="1">
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="62.25">
       <c r="A65" s="8">
         <v>44668.57983796296</v>
       </c>
@@ -10727,7 +10721,7 @@
       <c r="AY65" s="3"/>
       <c r="AZ65" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="17.25" hidden="1">
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="28.5">
       <c r="A66" s="8">
         <v>44668.99930555555</v>
       </c>
@@ -13703,7 +13697,7 @@
       <c r="AY102" s="3"/>
       <c r="AZ102" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="59.4" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A103" s="2">
         <v>44658.07016203704</v>
       </c>
@@ -13803,7 +13797,7 @@
       <c r="AY103" s="3"/>
       <c r="AZ103" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="59.4" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A104" s="2">
         <v>44661.6728125</v>
       </c>
@@ -13887,7 +13881,7 @@
       <c r="AY104" s="3"/>
       <c r="AZ104" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="59.4" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A105" s="2">
         <v>44661.85538194444</v>
       </c>
@@ -13971,7 +13965,7 @@
       <c r="AY105" s="3"/>
       <c r="AZ105" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="59.4" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A106" s="2">
         <v>44661.93817129629</v>
       </c>
@@ -14055,7 +14049,7 @@
       <c r="AY106" s="3"/>
       <c r="AZ106" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="59.4" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A107" s="2">
         <v>44662.281018518515</v>
       </c>
@@ -14139,7 +14133,7 @@
       <c r="AY107" s="3"/>
       <c r="AZ107" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="59.4" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A108" s="2">
         <v>44662.48496527778</v>
       </c>
@@ -14223,7 +14217,7 @@
       <c r="AY108" s="3"/>
       <c r="AZ108" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="59.4" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A109" s="2">
         <v>44662.59679398148</v>
       </c>
@@ -14307,7 +14301,7 @@
       <c r="AY109" s="3"/>
       <c r="AZ109" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="59.4" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A110" s="2">
         <v>44662.682233796295</v>
       </c>
@@ -14389,7 +14383,7 @@
       <c r="AY110" s="3"/>
       <c r="AZ110" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="59.4" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A111" s="2">
         <v>44662.8637962963</v>
       </c>
@@ -14471,7 +14465,7 @@
       <c r="AY111" s="3"/>
       <c r="AZ111" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="59.4" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A112" s="2">
         <v>44663.461180555554</v>
       </c>
@@ -14555,7 +14549,7 @@
       <c r="AY112" s="3"/>
       <c r="AZ112" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="59.4" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A113" s="2">
         <v>44663.43962962963</v>
       </c>
@@ -14637,7 +14631,7 @@
       <c r="AY113" s="3"/>
       <c r="AZ113" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="59.4" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A114" s="2">
         <v>44663.7472337963</v>
       </c>
@@ -14721,7 +14715,7 @@
       <c r="AY114" s="3"/>
       <c r="AZ114" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="59.4" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A115" s="2">
         <v>44663.90487268518</v>
       </c>
@@ -14799,7 +14793,7 @@
       <c r="AY115" s="3"/>
       <c r="AZ115" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="59.4" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A116" s="2">
         <v>44663.913935185185</v>
       </c>
@@ -14877,7 +14871,7 @@
       <c r="AY116" s="3"/>
       <c r="AZ116" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="59.4" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A117" s="2">
         <v>44663.94894675926</v>
       </c>
@@ -14959,7 +14953,7 @@
       <c r="AY117" s="3"/>
       <c r="AZ117" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="59.4" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A118" s="2">
         <v>44664.04039351852</v>
       </c>
@@ -15043,7 +15037,7 @@
       <c r="AY118" s="3"/>
       <c r="AZ118" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="59.4" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A119" s="2">
         <v>44664.49085648148</v>
       </c>
@@ -15123,7 +15117,7 @@
       <c r="AY119" s="3"/>
       <c r="AZ119" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="59.4" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A120" s="2">
         <v>44664.63363425926</v>
       </c>
@@ -15201,7 +15195,7 @@
       <c r="AY120" s="3"/>
       <c r="AZ120" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="59.4" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A121" s="2">
         <v>44664.80626157407</v>
       </c>
@@ -15277,7 +15271,7 @@
       <c r="AY121" s="3"/>
       <c r="AZ121" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="59.4" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A122" s="2">
         <v>44664.95061342593</v>
       </c>
@@ -15361,7 +15355,7 @@
       <c r="AY122" s="3"/>
       <c r="AZ122" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="59.4" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A123" s="2">
         <v>44665.001909722225</v>
       </c>
@@ -15437,7 +15431,7 @@
       <c r="AY123" s="3"/>
       <c r="AZ123" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="59.4" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A124" s="2">
         <v>44665.37673611111</v>
       </c>
@@ -15521,7 +15515,7 @@
       <c r="AY124" s="3"/>
       <c r="AZ124" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="59.4" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A125" s="2">
         <v>44665.540810185186</v>
       </c>
@@ -15605,7 +15599,7 @@
       <c r="AY125" s="3"/>
       <c r="AZ125" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="59.4" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A126" s="2">
         <v>44666.08244212963</v>
       </c>
@@ -15679,7 +15673,7 @@
       <c r="AY126" s="3"/>
       <c r="AZ126" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="59.4" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A127" s="2">
         <v>44666.64837962963</v>
       </c>
@@ -15759,7 +15753,7 @@
       <c r="AY127" s="3"/>
       <c r="AZ127" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="59.4" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A128" s="2">
         <v>44667.49961805555</v>
       </c>
@@ -15843,7 +15837,7 @@
       <c r="AY128" s="3"/>
       <c r="AZ128" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="59.4">
+    <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="17.25" hidden="1">
       <c r="A129" s="8">
         <v>44668.54368055556</v>
       </c>
@@ -15927,7 +15921,7 @@
       <c r="AY129" s="3"/>
       <c r="AZ129" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="59.4">
+    <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="17.25" hidden="1">
       <c r="A130" s="8">
         <v>44668.84097222222</v>
       </c>
@@ -16009,7 +16003,7 @@
       <c r="AY130" s="3"/>
       <c r="AZ130" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="59.4">
+    <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="17.25" hidden="1">
       <c r="A131" s="8">
         <v>44668.8571875</v>
       </c>
@@ -16093,7 +16087,7 @@
       <c r="AY131" s="14"/>
       <c r="AZ131" s="14"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="59.4">
+    <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="17.25" hidden="1">
       <c r="A132" s="8">
         <v>44668.97381944444</v>
       </c>

</xml_diff>

<commit_message>
clustering: add identity mapping for supervised set
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -4936,7 +4936,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="18" width="18.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="19" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="19" width="23.290714285714284" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="19" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="19" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="19" width="12.43357142857143" customWidth="1" bestFit="1"/>
@@ -4948,11 +4948,11 @@
     <col min="11" max="11" style="20" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="12" max="12" style="19" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="13" max="13" style="19" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="19" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="19" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="19" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="19" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="19" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="19" width="44.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="19" width="47.005" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="19" width="40.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="19" width="30.005" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="19" width="31.862142857142857" customWidth="1" bestFit="1"/>
     <col min="19" max="19" style="19" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="20" max="20" style="19" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="21" max="21" style="19" width="12.43357142857143" customWidth="1" bestFit="1"/>
@@ -5133,7 +5133,7 @@
       <c r="AY1" s="3"/>
       <c r="AZ1" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A2" s="2">
         <v>44661.85490740741</v>
       </c>
@@ -5219,7 +5219,7 @@
       <c r="AY2" s="3"/>
       <c r="AZ2" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A3" s="2">
         <v>44661.87332175926</v>
       </c>
@@ -5311,7 +5311,7 @@
       <c r="AY3" s="3"/>
       <c r="AZ3" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A4" s="2">
         <v>44661.88621527778</v>
       </c>
@@ -5403,7 +5403,7 @@
       <c r="AY4" s="3"/>
       <c r="AZ4" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A5" s="2">
         <v>44661.9225</v>
       </c>
@@ -5493,7 +5493,7 @@
       <c r="AY5" s="3"/>
       <c r="AZ5" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A6" s="2">
         <v>44662.950277777774</v>
       </c>
@@ -5585,7 +5585,7 @@
       <c r="AY6" s="3"/>
       <c r="AZ6" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A7" s="2">
         <v>44661.95269675926</v>
       </c>
@@ -5677,7 +5677,7 @@
       <c r="AY7" s="3"/>
       <c r="AZ7" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A8" s="2">
         <v>44661.979363425926</v>
       </c>
@@ -5769,7 +5769,7 @@
       <c r="AY8" s="3"/>
       <c r="AZ8" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A9" s="2">
         <v>44661.98532407408</v>
       </c>
@@ -5861,7 +5861,7 @@
       <c r="AY9" s="3"/>
       <c r="AZ9" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A10" s="2">
         <v>44662.352627314816</v>
       </c>
@@ -5949,7 +5949,7 @@
       <c r="AY10" s="3"/>
       <c r="AZ10" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A11" s="2">
         <v>44662.4525</v>
       </c>
@@ -6039,7 +6039,7 @@
       <c r="AY11" s="3"/>
       <c r="AZ11" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A12" s="2">
         <v>44662.5453587963</v>
       </c>
@@ -6123,7 +6123,7 @@
       <c r="AY12" s="3"/>
       <c r="AZ12" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A13" s="2">
         <v>44662.83082175926</v>
       </c>
@@ -6215,7 +6215,7 @@
       <c r="AY13" s="3"/>
       <c r="AZ13" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A14" s="2">
         <v>44662.86724537037</v>
       </c>
@@ -6305,7 +6305,7 @@
       <c r="AY14" s="3"/>
       <c r="AZ14" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A15" s="2">
         <v>44662.87091435185</v>
       </c>
@@ -6397,7 +6397,7 @@
       <c r="AY15" s="3"/>
       <c r="AZ15" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A16" s="2">
         <v>44662.88334490741</v>
       </c>
@@ -6489,7 +6489,7 @@
       <c r="AY16" s="3"/>
       <c r="AZ16" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A17" s="2">
         <v>44662.932442129626</v>
       </c>
@@ -6575,7 +6575,7 @@
       <c r="AY17" s="3"/>
       <c r="AZ17" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A18" s="2">
         <v>44662.94488425926</v>
       </c>
@@ -6667,7 +6667,7 @@
       <c r="AY18" s="3"/>
       <c r="AZ18" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A19" s="2">
         <v>44662.9487037037</v>
       </c>
@@ -6755,7 +6755,7 @@
       <c r="AY19" s="3"/>
       <c r="AZ19" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A20" s="2">
         <v>44663.49254629629</v>
       </c>
@@ -6847,7 +6847,7 @@
       <c r="AY20" s="3"/>
       <c r="AZ20" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A21" s="2">
         <v>44663.658738425926</v>
       </c>
@@ -6939,7 +6939,7 @@
       <c r="AY21" s="3"/>
       <c r="AZ21" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A22" s="2">
         <v>44663.77224537037</v>
       </c>
@@ -7031,7 +7031,7 @@
       <c r="AY22" s="3"/>
       <c r="AZ22" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A23" s="2">
         <v>44663.95140046296</v>
       </c>
@@ -7123,7 +7123,7 @@
       <c r="AY23" s="3"/>
       <c r="AZ23" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A24" s="2">
         <v>44663.993576388886</v>
       </c>
@@ -7215,7 +7215,7 @@
       <c r="AY24" s="3"/>
       <c r="AZ24" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A25" s="2">
         <v>44663.99984953704</v>
       </c>
@@ -7307,7 +7307,7 @@
       <c r="AY25" s="3"/>
       <c r="AZ25" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A26" s="2">
         <v>44664.03806712963</v>
       </c>
@@ -7397,7 +7397,7 @@
       <c r="AY26" s="3"/>
       <c r="AZ26" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A27" s="2">
         <v>44664.41658564815</v>
       </c>
@@ -7489,7 +7489,7 @@
       <c r="AY27" s="3"/>
       <c r="AZ27" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A28" s="2">
         <v>44663.61819444445</v>
       </c>
@@ -7573,7 +7573,7 @@
       <c r="AY28" s="3"/>
       <c r="AZ28" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A29" s="2">
         <v>44664.75050925926</v>
       </c>
@@ -7665,7 +7665,7 @@
       <c r="AY29" s="3"/>
       <c r="AZ29" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A30" s="2">
         <v>44664.77416666667</v>
       </c>
@@ -7757,7 +7757,7 @@
       <c r="AY30" s="3"/>
       <c r="AZ30" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A31" s="2">
         <v>44664.93570601852</v>
       </c>
@@ -7849,7 +7849,7 @@
       <c r="AY31" s="3"/>
       <c r="AZ31" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A32" s="2">
         <v>44665.84037037037</v>
       </c>
@@ -7939,7 +7939,7 @@
       <c r="AY32" s="3"/>
       <c r="AZ32" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A33" s="2">
         <v>44666.962789351855</v>
       </c>
@@ -8031,7 +8031,7 @@
       <c r="AY33" s="3"/>
       <c r="AZ33" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A34" s="2">
         <v>44667.11704861111</v>
       </c>
@@ -8123,7 +8123,7 @@
       <c r="AY34" s="3"/>
       <c r="AZ34" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A35" s="2">
         <v>44667.86420138889</v>
       </c>
@@ -8213,7 +8213,7 @@
       <c r="AY35" s="3"/>
       <c r="AZ35" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A36" s="2">
         <v>44667.948159722226</v>
       </c>
@@ -8301,7 +8301,7 @@
       <c r="AY36" s="3"/>
       <c r="AZ36" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A37" s="2">
         <v>44667.99630787037</v>
       </c>
@@ -8391,7 +8391,7 @@
       <c r="AY37" s="3"/>
       <c r="AZ37" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A38" s="2">
         <v>44668.03163194445</v>
       </c>
@@ -8477,7 +8477,7 @@
       <c r="AY38" s="3"/>
       <c r="AZ38" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25" hidden="1">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25">
       <c r="A39" s="8">
         <v>44668.883206018516</v>
       </c>
@@ -8569,7 +8569,7 @@
       <c r="AY39" s="3"/>
       <c r="AZ39" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="17.25" hidden="1">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="17.25">
       <c r="A40" s="8">
         <v>44668.911782407406</v>
       </c>
@@ -8661,7 +8661,7 @@
       <c r="AY40" s="3"/>
       <c r="AZ40" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="17.25" hidden="1">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="17.25">
       <c r="A41" s="8">
         <v>44668.93439814815</v>
       </c>
@@ -8753,7 +8753,7 @@
       <c r="AY41" s="3"/>
       <c r="AZ41" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="17.25" hidden="1">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="17.25">
       <c r="A42" s="8">
         <v>44668.939409722225</v>
       </c>
@@ -8839,7 +8839,7 @@
       <c r="AY42" s="3"/>
       <c r="AZ42" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="377.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A43" s="2">
         <v>44661.87734953704</v>
       </c>
@@ -8921,7 +8921,7 @@
       <c r="AY43" s="3"/>
       <c r="AZ43" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="253.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A44" s="2">
         <v>44661.88207175926</v>
       </c>
@@ -9003,7 +9003,7 @@
       <c r="AY44" s="3"/>
       <c r="AZ44" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="467.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A45" s="2">
         <v>44661.89346064815</v>
       </c>
@@ -9085,7 +9085,7 @@
       <c r="AY45" s="3"/>
       <c r="AZ45" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="332.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A46" s="2">
         <v>44661.91300925926</v>
       </c>
@@ -9169,7 +9169,7 @@
       <c r="AY46" s="3"/>
       <c r="AZ46" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="107.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A47" s="2">
         <v>44661.99429398148</v>
       </c>
@@ -9253,7 +9253,7 @@
       <c r="AY47" s="3"/>
       <c r="AZ47" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="208.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A48" s="2">
         <v>44662.46576388889</v>
       </c>
@@ -9333,7 +9333,7 @@
       <c r="AY48" s="3"/>
       <c r="AZ48" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="107.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A49" s="2">
         <v>44662.556296296294</v>
       </c>
@@ -9415,7 +9415,7 @@
       <c r="AY49" s="3"/>
       <c r="AZ49" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="861" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A50" s="2">
         <v>44662.921747685185</v>
       </c>
@@ -9497,7 +9497,7 @@
       <c r="AY50" s="3"/>
       <c r="AZ50" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="591" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A51" s="2">
         <v>44663.46912037037</v>
       </c>
@@ -9579,7 +9579,7 @@
       <c r="AY51" s="3"/>
       <c r="AZ51" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="163.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A52" s="2">
         <v>44663.75908564815</v>
       </c>
@@ -9661,7 +9661,7 @@
       <c r="AY52" s="3"/>
       <c r="AZ52" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="557.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A53" s="2">
         <v>44663.89796296296</v>
       </c>
@@ -9741,7 +9741,7 @@
       <c r="AY53" s="3"/>
       <c r="AZ53" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="759.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A54" s="2">
         <v>44663.90766203704</v>
       </c>
@@ -9825,7 +9825,7 @@
       <c r="AY54" s="3"/>
       <c r="AZ54" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="141" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A55" s="2">
         <v>44663.916597222225</v>
       </c>
@@ -9907,7 +9907,7 @@
       <c r="AY55" s="3"/>
       <c r="AZ55" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="343.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A56" s="2">
         <v>44663.92427083333</v>
       </c>
@@ -9991,7 +9991,7 @@
       <c r="AY56" s="3"/>
       <c r="AZ56" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="197.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A57" s="2">
         <v>44664.02513888889</v>
       </c>
@@ -10075,7 +10075,7 @@
       <c r="AY57" s="3"/>
       <c r="AZ57" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="332.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A58" s="2">
         <v>44664.72607638889</v>
       </c>
@@ -10157,7 +10157,7 @@
       <c r="AY58" s="3"/>
       <c r="AZ58" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="366" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A59" s="2">
         <v>44664.75571759259</v>
       </c>
@@ -10241,7 +10241,7 @@
       <c r="AY59" s="3"/>
       <c r="AZ59" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="748.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A60" s="2">
         <v>44664.803125</v>
       </c>
@@ -10325,7 +10325,7 @@
       <c r="AY60" s="3"/>
       <c r="AZ60" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="613.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A61" s="2">
         <v>44664.999710648146</v>
       </c>
@@ -10401,7 +10401,7 @@
       <c r="AY61" s="3"/>
       <c r="AZ61" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="253.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A62" s="2">
         <v>44665.467453703706</v>
       </c>
@@ -10481,7 +10481,7 @@
       <c r="AY62" s="3"/>
       <c r="AZ62" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="242.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="17.25" customFormat="1" s="1" hidden="1">
       <c r="A63" s="2">
         <v>44667.02175925926</v>
       </c>
@@ -10563,7 +10563,7 @@
       <c r="AY63" s="3"/>
       <c r="AZ63" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="28.5">
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="17.25" hidden="1">
       <c r="A64" s="8">
         <v>44668.51908564815</v>
       </c>
@@ -10647,7 +10647,7 @@
       <c r="AY64" s="3"/>
       <c r="AZ64" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="62.25">
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="17.25" hidden="1">
       <c r="A65" s="8">
         <v>44668.57983796296</v>
       </c>
@@ -10721,7 +10721,7 @@
       <c r="AY65" s="3"/>
       <c r="AZ65" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="28.5">
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="17.25" hidden="1">
       <c r="A66" s="8">
         <v>44668.99930555555</v>
       </c>

</xml_diff>